<commit_message>
writing something for the report
</commit_message>
<xml_diff>
--- a/results/sub_genre/metriche_Fabio.xlsx
+++ b/results/sub_genre/metriche_Fabio.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code_GitHub\Python\LFN\Robe mie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code_GitHub\Python\LFN\lfn_project\results\sub_genre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342EE03C-DB1D-4C33-8814-F842BDBA3676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9641C3C2-7977-4231-952B-3A4FDB105779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{3B0FC85E-6C2D-4D99-B44C-E1F9E2BE52AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3B0FC85E-6C2D-4D99-B44C-E1F9E2BE52AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Pop</t>
   </si>
@@ -90,6 +90,39 @@
   </si>
   <si>
     <t>trap</t>
+  </si>
+  <si>
+    <t>classical</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>dance</t>
+  </si>
+  <si>
+    <t>dubstep</t>
+  </si>
+  <si>
+    <t>edm</t>
+  </si>
+  <si>
+    <t>folk</t>
+  </si>
+  <si>
+    <t>house</t>
+  </si>
+  <si>
+    <t>indie</t>
+  </si>
+  <si>
+    <t>j-pop</t>
+  </si>
+  <si>
+    <t>jazz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nodes </t>
   </si>
 </sst>
 </file>
@@ -125,8 +158,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -461,11 +495,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09CC142D-2A50-4469-82BC-4A38D45A8AF4}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +507,7 @@
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="4" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -760,7 +794,294 @@
         <v>13755</v>
       </c>
     </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>541</v>
+      </c>
+      <c r="C11">
+        <v>244</v>
+      </c>
+      <c r="D11">
+        <v>475</v>
+      </c>
+      <c r="E11">
+        <v>144</v>
+      </c>
+      <c r="F11">
+        <v>337</v>
+      </c>
+      <c r="G11">
+        <v>920</v>
+      </c>
+      <c r="H11">
+        <v>960</v>
+      </c>
+      <c r="I11">
+        <v>2243</v>
+      </c>
+      <c r="J11">
+        <v>162</v>
+      </c>
+      <c r="K11">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>1.3354997068175699E-3</v>
+      </c>
+      <c r="C12">
+        <v>3.2742498346054701E-2</v>
+      </c>
+      <c r="D12">
+        <v>0.109888508805515</v>
+      </c>
+      <c r="E12">
+        <v>8.5950241078218401E-2</v>
+      </c>
+      <c r="F12">
+        <v>0.12724174906165001</v>
+      </c>
+      <c r="G12">
+        <v>1.81759018759018E-2</v>
+      </c>
+      <c r="H12">
+        <v>8.6032234230052101E-2</v>
+      </c>
+      <c r="I12">
+        <v>1.6725473036037601E-2</v>
+      </c>
+      <c r="J12">
+        <v>2.2051209528523501E-2</v>
+      </c>
+      <c r="K12">
+        <v>1.1661246587032201E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1">
+        <v>8.7678919795708101E-5</v>
+      </c>
+      <c r="C13">
+        <v>5.6603773584905599E-2</v>
+      </c>
+      <c r="D13">
+        <v>0.107765417149428</v>
+      </c>
+      <c r="E13">
+        <v>4.6349089571454803E-2</v>
+      </c>
+      <c r="F13">
+        <v>0.110340237265573</v>
+      </c>
+      <c r="G13">
+        <v>7.6988879384088896E-2</v>
+      </c>
+      <c r="H13">
+        <v>7.0883399725723203E-2</v>
+      </c>
+      <c r="I13">
+        <v>4.5769346582354702E-2</v>
+      </c>
+      <c r="J13">
+        <v>9.8786828422876893E-2</v>
+      </c>
+      <c r="K13">
+        <v>2.7067669172932299E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>1E-4</v>
+      </c>
+      <c r="C14">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="D14">
+        <v>0.1129</v>
+      </c>
+      <c r="E14">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F14">
+        <v>0.1082</v>
+      </c>
+      <c r="G14">
+        <v>6.9900000000000004E-2</v>
+      </c>
+      <c r="I14">
+        <v>4.4299999999999999E-2</v>
+      </c>
+      <c r="J14">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="K14">
+        <v>2.5600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15">
+        <v>1260</v>
+      </c>
+      <c r="C15">
+        <v>530</v>
+      </c>
+      <c r="D15">
+        <v>2210</v>
+      </c>
+      <c r="E15">
+        <v>351</v>
+      </c>
+      <c r="F15">
+        <v>1346</v>
+      </c>
+      <c r="G15">
+        <v>1250</v>
+      </c>
+      <c r="H15">
+        <v>3249</v>
+      </c>
+      <c r="I15">
+        <v>3860</v>
+      </c>
+      <c r="J15">
+        <v>290</v>
+      </c>
+      <c r="K15">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>775</v>
+      </c>
+      <c r="C16">
+        <v>441</v>
+      </c>
+      <c r="D16">
+        <v>8190</v>
+      </c>
+      <c r="E16">
+        <v>331</v>
+      </c>
+      <c r="F16">
+        <v>4568</v>
+      </c>
+      <c r="G16">
+        <v>372</v>
+      </c>
+      <c r="H16">
+        <v>8187</v>
+      </c>
+      <c r="I16">
+        <v>2052</v>
+      </c>
+      <c r="J16">
+        <v>165</v>
+      </c>
+      <c r="K16">
+        <v>421</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="D4:M4">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:M4">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:M4 B13:K13">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:M3 B12:K12">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>